<commit_message>
pull z interfacem do dodawania uczestnika
</commit_message>
<xml_diff>
--- a/docs/assets/kr2018.xlsx
+++ b/docs/assets/kr2018.xlsx
@@ -2652,9 +2652,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="19" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="19" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -6006,7 +6006,7 @@
   </sheetPr>
   <dimension ref="A1:Y1540"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A514" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -6273,7 +6273,7 @@
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
     </row>
-    <row r="7" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="59"/>
       <c r="B7" s="60" t="str">
         <f aca="false">B1</f>

</xml_diff>